<commit_message>
Development : Entity and Repository setting complete
</commit_message>
<xml_diff>
--- a/DBMS_논리적설계.xlsx
+++ b/DBMS_논리적설계.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shin Min Gee\Desktop\adminPage_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EE5266-8B48-44F0-85AB-FAFB2AAA1814}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E9D9F7-E5F9-49F8-AE42-0982E765255A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{6AE60926-0586-4163-ADC3-4FDAEA24E71A}"/>
+    <workbookView xWindow="4800" yWindow="2240" windowWidth="14400" windowHeight="8560" xr2:uid="{6AE60926-0586-4163-ADC3-4FDAEA24E71A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C510AB61-7025-4CB9-89C7-7D6DD6B8EB4D}" name="표1" displayName="표1" ref="B3:D10" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C510AB61-7025-4CB9-89C7-7D6DD6B8EB4D}" name="표1" displayName="표1" ref="B3:D10" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="B3:D10" xr:uid="{904B5523-412F-4847-A9CE-F72C8B6342DD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -625,7 +625,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9EC0B675-42C8-4882-AFD7-CCAEF1C3CD56}" name="표1_3" displayName="표1_3" ref="B19:D31" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9EC0B675-42C8-4882-AFD7-CCAEF1C3CD56}" name="표1_3" displayName="표1_3" ref="B19:D31" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="B19:D31" xr:uid="{05F82C2A-44F1-42D2-B584-08B0BA0731EA}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1019,7 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107B5FBF-91E5-40EE-BBD4-C8B0B0E92407}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
@@ -1031,7 +1031,7 @@
     <col min="6" max="6" width="15.9140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Development : Controller with enumclass & Service Logic complete
</commit_message>
<xml_diff>
--- a/DBMS_논리적설계.xlsx
+++ b/DBMS_논리적설계.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shin Min Gee\Desktop\adminPage_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B342A7-CD47-483D-A1E1-A8A8ECFF005F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED176C73-3776-482D-A084-0BEADA1C4328}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-820" yWindow="870" windowWidth="13180" windowHeight="8560" xr2:uid="{6AE60926-0586-4163-ADC3-4FDAEA24E71A}"/>
+    <workbookView xWindow="20" yWindow="640" windowWidth="11170" windowHeight="8560" xr2:uid="{6AE60926-0586-4163-ADC3-4FDAEA24E71A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1044,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107B5FBF-91E5-40EE-BBD4-C8B0B0E92407}">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -1060,7 +1060,8 @@
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.75" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>